<commit_message>
Individuals admin add/update iban from xlsx
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/household/tests/test_file/iban_update_invalid_no_match.xlsx
+++ b/backend/hct_mis_api/apps/household/tests/test_file/iban_update_invalid_no_match.xlsx
@@ -19,7 +19,7 @@
     <t>IBAN</t>
   </si>
   <si>
-    <t>Last Status</t>
+    <t>BANK_NAME</t>
   </si>
   <si>
     <t>Timestamp</t>
@@ -31,7 +31,7 @@
     <t>111</t>
   </si>
   <si>
-    <t>Delivered</t>
+    <t>Super Bank</t>
   </si>
   <si>
     <t>rejected fasdas some decription n</t>
@@ -40,7 +40,7 @@
     <t>222</t>
   </si>
   <si>
-    <t>FAILED</t>
+    <t>Bank</t>
   </si>
   <si>
     <t>rejejeje descreerer</t>

</xml_diff>

<commit_message>
Individuals admin add/update iban from xlsx (#1675)
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/household/tests/test_file/iban_update_invalid_no_match.xlsx
+++ b/backend/hct_mis_api/apps/household/tests/test_file/iban_update_invalid_no_match.xlsx
@@ -19,7 +19,7 @@
     <t>IBAN</t>
   </si>
   <si>
-    <t>Last Status</t>
+    <t>BANK_NAME</t>
   </si>
   <si>
     <t>Timestamp</t>
@@ -31,7 +31,7 @@
     <t>111</t>
   </si>
   <si>
-    <t>Delivered</t>
+    <t>Super Bank</t>
   </si>
   <si>
     <t>rejected fasdas some decription n</t>
@@ -40,7 +40,7 @@
     <t>222</t>
   </si>
   <si>
-    <t>FAILED</t>
+    <t>Bank</t>
   </si>
   <si>
     <t>rejejeje descreerer</t>

</xml_diff>

<commit_message>
Individuals admin add/update iban from xlsx AB#125503
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/household/tests/test_file/iban_update_invalid_no_match.xlsx
+++ b/backend/hct_mis_api/apps/household/tests/test_file/iban_update_invalid_no_match.xlsx
@@ -19,7 +19,7 @@
     <t>IBAN</t>
   </si>
   <si>
-    <t>Last Status</t>
+    <t>BANK_NAME</t>
   </si>
   <si>
     <t>Timestamp</t>
@@ -31,7 +31,7 @@
     <t>111</t>
   </si>
   <si>
-    <t>Delivered</t>
+    <t>Super Bank</t>
   </si>
   <si>
     <t>rejected fasdas some decription n</t>
@@ -40,7 +40,7 @@
     <t>222</t>
   </si>
   <si>
-    <t>FAILED</t>
+    <t>Bank</t>
   </si>
   <si>
     <t>rejejeje descreerer</t>

</xml_diff>

<commit_message>
Rebase payment module (#1737)
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/household/tests/test_file/iban_update_invalid_no_match.xlsx
+++ b/backend/hct_mis_api/apps/household/tests/test_file/iban_update_invalid_no_match.xlsx
@@ -19,7 +19,7 @@
     <t>IBAN</t>
   </si>
   <si>
-    <t>Last Status</t>
+    <t>BANK_NAME</t>
   </si>
   <si>
     <t>Timestamp</t>
@@ -31,7 +31,7 @@
     <t>111</t>
   </si>
   <si>
-    <t>Delivered</t>
+    <t>Super Bank</t>
   </si>
   <si>
     <t>rejected fasdas some decription n</t>
@@ -40,7 +40,7 @@
     <t>222</t>
   </si>
   <si>
-    <t>FAILED</t>
+    <t>Bank</t>
   </si>
   <si>
     <t>rejejeje descreerer</t>

</xml_diff>